<commit_message>
real name of student
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\Developper\web0\7s\API and Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B81F2AE-0984-42ED-9A6C-13DFF0090F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD5A2A-4431-4B1C-B680-FF5720A50E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,82 +30,82 @@
     <t>id</t>
   </si>
   <si>
-    <t>student1</t>
-  </si>
-  <si>
-    <t>student2</t>
-  </si>
-  <si>
-    <t>student3</t>
-  </si>
-  <si>
-    <t>student4</t>
-  </si>
-  <si>
-    <t>student5</t>
-  </si>
-  <si>
-    <t>student6</t>
-  </si>
-  <si>
-    <t>student7</t>
-  </si>
-  <si>
-    <t>student8</t>
-  </si>
-  <si>
-    <t>student9</t>
-  </si>
-  <si>
-    <t>student10</t>
-  </si>
-  <si>
-    <t>student11</t>
-  </si>
-  <si>
-    <t>student12</t>
-  </si>
-  <si>
-    <t>student13</t>
-  </si>
-  <si>
-    <t>student14</t>
-  </si>
-  <si>
-    <t>student15</t>
-  </si>
-  <si>
-    <t>student16</t>
-  </si>
-  <si>
-    <t>student17</t>
-  </si>
-  <si>
-    <t>student18</t>
-  </si>
-  <si>
-    <t>student19</t>
-  </si>
-  <si>
-    <t>student20</t>
-  </si>
-  <si>
-    <t>student21</t>
-  </si>
-  <si>
-    <t>student22</t>
-  </si>
-  <si>
-    <t>student23</t>
-  </si>
-  <si>
-    <t>student24</t>
-  </si>
-  <si>
-    <t>student25</t>
-  </si>
-  <si>
     <t>names</t>
+  </si>
+  <si>
+    <t>wael</t>
+  </si>
+  <si>
+    <t>brahim</t>
+  </si>
+  <si>
+    <t>Rony</t>
+  </si>
+  <si>
+    <t>razane</t>
+  </si>
+  <si>
+    <t>lina</t>
+  </si>
+  <si>
+    <t>josian</t>
+  </si>
+  <si>
+    <t>zeina</t>
+  </si>
+  <si>
+    <t>sirine</t>
+  </si>
+  <si>
+    <t>abd</t>
+  </si>
+  <si>
+    <t>omar</t>
+  </si>
+  <si>
+    <t>imad</t>
+  </si>
+  <si>
+    <t>abd2</t>
+  </si>
+  <si>
+    <t>patricia</t>
+  </si>
+  <si>
+    <t>joumana</t>
+  </si>
+  <si>
+    <t>sami</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>hadi</t>
+  </si>
+  <si>
+    <t>ziad</t>
+  </si>
+  <si>
+    <t>nadim</t>
+  </si>
+  <si>
+    <t>ahmad</t>
+  </si>
+  <si>
+    <t>samir</t>
+  </si>
+  <si>
+    <t>fatima</t>
+  </si>
+  <si>
+    <t>jad</t>
+  </si>
+  <si>
+    <t>jihad</t>
+  </si>
+  <si>
+    <t>bilal</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -482,7 +482,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -498,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -522,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -538,7 +538,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -546,7 +546,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -562,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -578,7 +578,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -586,7 +586,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -618,7 +618,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -634,7 +634,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>